<commit_message>
produce predicted probabilities of transitlities of being inactive using ukhls
</commit_message>
<xml_diff>
--- a/data/economic_activities_categories.xlsx
+++ b/data/economic_activities_categories.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonMinton/repos/economic_inactivity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440ADA36-C1DD-464A-9D4E-41BDF438A074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F06AE4-9C72-E041-ABCB-548A043A4361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D9F6BCC1-9FE2-2642-9ABB-795D26BAAAE2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{D9F6BCC1-9FE2-2642-9ABB-795D26BAAAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
   <si>
     <t xml:space="preserve">Family care or home                    </t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Temporarily laid off/short term working</t>
-  </si>
-  <si>
-    <t>Family care or home</t>
   </si>
 </sst>
 </file>
@@ -540,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3B8471-D57B-8943-BAF1-C3BDD3150CF4}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" workbookViewId="0">
+      <selection activeCell="A43" sqref="A26:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,23 +976,6 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
look at econ activity status over time and age group and sex; produce prelim report
</commit_message>
<xml_diff>
--- a/data/economic_activities_categories.xlsx
+++ b/data/economic_activities_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonMinton/repos/economic_inactivity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F06AE4-9C72-E041-ABCB-548A043A4361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7155AEDE-0FF4-B244-A2F1-DAF10584B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{D9F6BCC1-9FE2-2642-9ABB-795D26BAAAE2}"/>
   </bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3B8471-D57B-8943-BAF1-C3BDD3150CF4}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" workbookViewId="0">
-      <selection activeCell="A43" sqref="A26:XFD43"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,7 +800,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>

</xml_diff>